<commit_message>
Corrected site names that did not match either DOVS or UVC data
</commit_message>
<xml_diff>
--- a/Data/SiteKeys.xlsx
+++ b/Data/SiteKeys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denisse\Documents\Work\Sara\UVC_DOVS_Galapagos\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2838EEED-6107-4A3C-BDD3-8F9F7FC7BE78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FB96F8-2486-4516-ABC1-4E0497D590FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{520C0315-4934-4420-8948-D1D1C72D6F66}"/>
   </bookViews>
@@ -1255,7 +1255,7 @@
   <dimension ref="A1:F986"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>